<commit_message>
extract variables from data sets
</commit_message>
<xml_diff>
--- a/Variable definition.xlsx
+++ b/Variable definition.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="154">
   <si>
     <t>Population</t>
   </si>
@@ -379,6 +379,114 @@
   </si>
   <si>
     <t>Income in the past 12 months below poverty level</t>
+  </si>
+  <si>
+    <t>Household income</t>
+  </si>
+  <si>
+    <t>Less than $10,000</t>
+  </si>
+  <si>
+    <t>B19001_002E</t>
+  </si>
+  <si>
+    <t>$10,000 to $14,999</t>
+  </si>
+  <si>
+    <t>$15,000 to $19,999</t>
+  </si>
+  <si>
+    <t>$20,000 to $24,999</t>
+  </si>
+  <si>
+    <t>$25,000 to $29,999</t>
+  </si>
+  <si>
+    <t>$30,000 to $34,999</t>
+  </si>
+  <si>
+    <t>$35,000 to $39,999</t>
+  </si>
+  <si>
+    <t>$40,000 to $44,999</t>
+  </si>
+  <si>
+    <t>$45,000 to $49,999</t>
+  </si>
+  <si>
+    <t>$50,000 to $59,999</t>
+  </si>
+  <si>
+    <t>$60,000 to $74,999</t>
+  </si>
+  <si>
+    <t>B19001_004E</t>
+  </si>
+  <si>
+    <t>B19001_003E</t>
+  </si>
+  <si>
+    <t>B19001_006E</t>
+  </si>
+  <si>
+    <t>B19001_005E</t>
+  </si>
+  <si>
+    <t>B19001_007E</t>
+  </si>
+  <si>
+    <t>B19001_008E</t>
+  </si>
+  <si>
+    <t>B19001_009E</t>
+  </si>
+  <si>
+    <t>B19001_010E</t>
+  </si>
+  <si>
+    <t>B19001_011E</t>
+  </si>
+  <si>
+    <t>B19001_012E</t>
+  </si>
+  <si>
+    <t>$75,000 to $99,999</t>
+  </si>
+  <si>
+    <t>B19001_013E</t>
+  </si>
+  <si>
+    <t>$100,000 to $124,999</t>
+  </si>
+  <si>
+    <t>B19001_014E</t>
+  </si>
+  <si>
+    <t>$125,000 to $149,999</t>
+  </si>
+  <si>
+    <t>B19001_015E</t>
+  </si>
+  <si>
+    <t>$150,000 to $199,999</t>
+  </si>
+  <si>
+    <t>B19001_016E</t>
+  </si>
+  <si>
+    <t>$200,000 or more</t>
+  </si>
+  <si>
+    <t>Employment status for the population 16 years and over</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In labor force; Civilian labor force; Unemployed</t>
+  </si>
+  <si>
+    <t>B23025_005E</t>
+  </si>
+  <si>
+    <t>B19001_017E</t>
   </si>
 </sst>
 </file>
@@ -764,8 +872,8 @@
   <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -775,7 +883,7 @@
     <col min="3" max="3" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -786,12 +894,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
         <v>75</v>
       </c>
@@ -799,105 +907,141 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="B7" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="B10" t="s">
         <v>23</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="B11" t="s">
         <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="B12" t="s">
         <v>25</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="B14" t="s">
         <v>27</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="B15" t="s">
         <v>28</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="B16" t="s">
         <v>29</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:13">
@@ -906,6 +1050,9 @@
       </c>
       <c r="C17" t="s">
         <v>78</v>
+      </c>
+      <c r="D17">
+        <v>13</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
@@ -924,6 +1071,9 @@
       <c r="C18" t="s">
         <v>80</v>
       </c>
+      <c r="D18">
+        <v>14</v>
+      </c>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -941,6 +1091,9 @@
       <c r="C19" t="s">
         <v>82</v>
       </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -958,6 +1111,9 @@
       <c r="C20" t="s">
         <v>84</v>
       </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
       <c r="E20" s="3"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -975,6 +1131,9 @@
       <c r="C21" t="s">
         <v>86</v>
       </c>
+      <c r="D21">
+        <v>17</v>
+      </c>
       <c r="E21" s="3"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -992,6 +1151,9 @@
       <c r="C22" t="s">
         <v>88</v>
       </c>
+      <c r="D22">
+        <v>18</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1009,6 +1171,9 @@
       <c r="C23" t="s">
         <v>90</v>
       </c>
+      <c r="D23">
+        <v>19</v>
+      </c>
       <c r="E23" s="3"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1026,6 +1191,9 @@
       <c r="C24" t="s">
         <v>92</v>
       </c>
+      <c r="D24">
+        <v>20</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1043,6 +1211,9 @@
       <c r="C25" t="s">
         <v>94</v>
       </c>
+      <c r="D25">
+        <v>21</v>
+      </c>
       <c r="E25" s="3"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1060,6 +1231,9 @@
       <c r="C26" t="s">
         <v>96</v>
       </c>
+      <c r="D26">
+        <v>22</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1077,6 +1251,9 @@
       <c r="C27" t="s">
         <v>98</v>
       </c>
+      <c r="D27">
+        <v>23</v>
+      </c>
       <c r="E27" s="3"/>
       <c r="F27" s="2"/>
     </row>
@@ -1087,6 +1264,9 @@
       <c r="C29" t="s">
         <v>18</v>
       </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="2:13">
       <c r="B30" t="s">
@@ -1095,6 +1275,9 @@
       <c r="C30" t="s">
         <v>19</v>
       </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="2:13">
       <c r="B31" t="s">
@@ -1103,6 +1286,9 @@
       <c r="C31" t="s">
         <v>31</v>
       </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="2:13">
       <c r="B32" t="s">
@@ -1111,165 +1297,225 @@
       <c r="C32" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="33" spans="2:3">
+      <c r="D32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4">
       <c r="B33" t="s">
         <v>34</v>
       </c>
       <c r="C33" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="34" spans="2:3">
+      <c r="D33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4">
       <c r="B34" t="s">
         <v>36</v>
       </c>
       <c r="C34" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="2:3">
+      <c r="D34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4">
       <c r="B35" t="s">
         <v>38</v>
       </c>
       <c r="C35" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="2:3">
+      <c r="D35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4">
       <c r="B36" t="s">
         <v>40</v>
       </c>
       <c r="C36" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="37" spans="2:3">
+      <c r="D36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4">
       <c r="B37" t="s">
         <v>42</v>
       </c>
       <c r="C37" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="38" spans="2:3">
+      <c r="D37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4">
       <c r="B38" t="s">
         <v>44</v>
       </c>
       <c r="C38" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="39" spans="2:3">
+      <c r="D38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4">
       <c r="B39" t="s">
         <v>46</v>
       </c>
       <c r="C39" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="40" spans="2:3">
+      <c r="D39">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4">
       <c r="B40" t="s">
         <v>48</v>
       </c>
       <c r="C40" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="41" spans="2:3">
+      <c r="D40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4">
       <c r="B41" t="s">
         <v>50</v>
       </c>
       <c r="C41" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="42" spans="2:3">
+      <c r="D41">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4">
       <c r="B42" t="s">
         <v>52</v>
       </c>
       <c r="C42" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="43" spans="2:3">
+      <c r="D42">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4">
       <c r="B43" t="s">
         <v>54</v>
       </c>
       <c r="C43" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="44" spans="2:3">
+      <c r="D43">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4">
       <c r="B44" t="s">
         <v>56</v>
       </c>
       <c r="C44" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="45" spans="2:3">
+      <c r="D44">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4">
       <c r="B45" t="s">
         <v>58</v>
       </c>
       <c r="C45" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="46" spans="2:3">
+      <c r="D45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4">
       <c r="B46" t="s">
         <v>60</v>
       </c>
       <c r="C46" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="47" spans="2:3">
+      <c r="D46">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4">
       <c r="B47" t="s">
         <v>62</v>
       </c>
       <c r="C47" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="48" spans="2:3">
+      <c r="D47">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4">
       <c r="B48" t="s">
         <v>64</v>
       </c>
       <c r="C48" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
+      <c r="D48">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="B49" t="s">
         <v>66</v>
       </c>
       <c r="C49" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
+      <c r="D49">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="B50" t="s">
         <v>68</v>
       </c>
       <c r="C50" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
+      <c r="D50">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="B51" t="s">
         <v>70</v>
       </c>
       <c r="C51" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
+      <c r="D51">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:4">
       <c r="B54" t="s">
         <v>103</v>
       </c>
@@ -1277,7 +1523,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:4">
       <c r="B55" t="s">
         <v>104</v>
       </c>
@@ -1285,7 +1531,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:4">
       <c r="B56" t="s">
         <v>105</v>
       </c>
@@ -1314,17 +1560,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30B2A30D-1C2E-EC47-BD57-5987F908EF61}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
-    <col min="3" max="3" width="41.33203125" customWidth="1"/>
+    <col min="3" max="3" width="56.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1">
@@ -1388,6 +1635,152 @@
         <v>117</v>
       </c>
     </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="B13" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="B14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" t="s">
+        <v>134</v>
+      </c>
+      <c r="C15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C16" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="B17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="B18" t="s">
+        <v>136</v>
+      </c>
+      <c r="C18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" t="s">
+        <v>137</v>
+      </c>
+      <c r="C19" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="B20" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="B21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C25" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="B27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="B30" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" t="s">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>